<commit_message>
simulation frameworks using the simmer package
</commit_message>
<xml_diff>
--- a/2021 data/2021 filtered/generation_21.xlsx
+++ b/2021 data/2021 filtered/generation_21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kovac\Desktop\Work\Green UP Project\green-up-project\2021 data\2021 filtered\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D652C84-3BC7-40C4-AB08-1A06E4969D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807E77C3-A11F-4392-A50C-9D1F467AC00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>15 01 01</t>
   </si>
   <si>
-    <t>Paper and cardboard packaging and cardboard packaging</t>
-  </si>
-  <si>
     <t>15 01 03</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>NEOPREDELJENO</t>
+  </si>
+  <si>
+    <t>Paper and cardboard packaging</t>
   </si>
 </sst>
 </file>
@@ -482,17 +482,17 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.453125" customWidth="1"/>
-    <col min="5" max="5" width="70.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -574,7 +574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -588,7 +588,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F3">
         <v>4397061</v>
@@ -615,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -626,10 +626,10 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>2499245</v>
@@ -656,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -667,10 +667,10 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
       <c r="F5">
         <v>83320</v>
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -708,10 +708,10 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
       </c>
       <c r="F6">
         <v>244960</v>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -787,13 +787,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>4869959.8</v>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -828,13 +828,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
       </c>
       <c r="F9">
         <v>1427842</v>
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -869,13 +869,13 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
         <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
       </c>
       <c r="F10">
         <v>90435</v>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -910,13 +910,13 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
         <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
       </c>
       <c r="F11">
         <v>63200</v>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -951,7 +951,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -992,13 +992,13 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F13">
         <v>5088934</v>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -1033,13 +1033,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
         <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
       </c>
       <c r="F14">
         <v>2254343</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -1074,13 +1074,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
         <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
       </c>
       <c r="F15">
         <v>252950</v>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -1115,13 +1115,13 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
         <v>23</v>
-      </c>
-      <c r="E16" t="s">
-        <v>24</v>
       </c>
       <c r="F16">
         <v>79569</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -1197,13 +1197,13 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F18">
         <v>1729062</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -1238,13 +1238,13 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
         <v>19</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
       </c>
       <c r="F19">
         <v>545475</v>
@@ -1271,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2021</v>
       </c>
@@ -1279,13 +1279,13 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
         <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>22</v>
       </c>
       <c r="F20">
         <v>9090</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2021</v>
       </c>
@@ -1320,13 +1320,13 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
         <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
       </c>
       <c r="F21">
         <v>46200</v>
@@ -1353,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -1394,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -1402,13 +1402,13 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F23">
         <v>1925269</v>
@@ -1435,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -1443,13 +1443,13 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
         <v>19</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
       </c>
       <c r="F24">
         <v>2004725</v>
@@ -1476,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2021</v>
       </c>
@@ -1484,13 +1484,13 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
         <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>22</v>
       </c>
       <c r="F25">
         <v>67942</v>
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2021</v>
       </c>
@@ -1525,13 +1525,13 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
         <v>23</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
       </c>
       <c r="F26">
         <v>35245</v>
@@ -1558,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -1607,13 +1607,13 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F28">
         <v>22160619</v>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2021</v>
       </c>
@@ -1648,13 +1648,13 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
         <v>19</v>
-      </c>
-      <c r="E29" t="s">
-        <v>20</v>
       </c>
       <c r="F29">
         <v>5186000</v>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -1689,13 +1689,13 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
         <v>21</v>
-      </c>
-      <c r="E30" t="s">
-        <v>22</v>
       </c>
       <c r="F30">
         <v>660541</v>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2021</v>
       </c>
@@ -1730,13 +1730,13 @@
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
         <v>23</v>
-      </c>
-      <c r="E31" t="s">
-        <v>24</v>
       </c>
       <c r="F31">
         <v>278067</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2021</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -1812,13 +1812,13 @@
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F33">
         <v>8289364</v>
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2021</v>
       </c>
@@ -1853,13 +1853,13 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
         <v>19</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
       </c>
       <c r="F34">
         <v>2768993</v>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -1894,13 +1894,13 @@
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
         <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>22</v>
       </c>
       <c r="F35">
         <v>102640</v>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2021</v>
       </c>
@@ -1935,13 +1935,13 @@
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
         <v>23</v>
-      </c>
-      <c r="E36" t="s">
-        <v>24</v>
       </c>
       <c r="F36">
         <v>721127</v>
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2021</v>
       </c>
@@ -1976,13 +1976,13 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
         <v>31</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>32</v>
-      </c>
-      <c r="E37" t="s">
-        <v>33</v>
       </c>
       <c r="F37">
         <v>148</v>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -2058,13 +2058,13 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F39">
         <v>2535629</v>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2021</v>
       </c>
@@ -2099,13 +2099,13 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
         <v>19</v>
-      </c>
-      <c r="E40" t="s">
-        <v>20</v>
       </c>
       <c r="F40">
         <v>735230</v>
@@ -2132,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2021</v>
       </c>
@@ -2140,13 +2140,13 @@
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
         <v>21</v>
-      </c>
-      <c r="E41" t="s">
-        <v>22</v>
       </c>
       <c r="F41">
         <v>163420</v>
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2021</v>
       </c>
@@ -2181,13 +2181,13 @@
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
         <v>23</v>
-      </c>
-      <c r="E42" t="s">
-        <v>24</v>
       </c>
       <c r="F42">
         <v>5180</v>
@@ -2214,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2021</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2021</v>
       </c>
@@ -2263,13 +2263,13 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F44">
         <v>1063619</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2021</v>
       </c>
@@ -2304,13 +2304,13 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" t="s">
         <v>19</v>
-      </c>
-      <c r="E45" t="s">
-        <v>20</v>
       </c>
       <c r="F45">
         <v>291665</v>
@@ -2337,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2021</v>
       </c>
@@ -2345,13 +2345,13 @@
         <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
         <v>21</v>
-      </c>
-      <c r="E46" t="s">
-        <v>22</v>
       </c>
       <c r="F46">
         <v>5160</v>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -2386,13 +2386,13 @@
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
         <v>23</v>
-      </c>
-      <c r="E47" t="s">
-        <v>24</v>
       </c>
       <c r="F47">
         <v>550250</v>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -2468,13 +2468,13 @@
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F49">
         <v>1315147</v>
@@ -2501,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2509,13 +2509,13 @@
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" t="s">
         <v>19</v>
-      </c>
-      <c r="E50" t="s">
-        <v>20</v>
       </c>
       <c r="F50">
         <v>348176</v>
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2550,13 +2550,13 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
         <v>21</v>
-      </c>
-      <c r="E51" t="s">
-        <v>22</v>
       </c>
       <c r="F51">
         <v>85120</v>
@@ -2583,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2591,13 +2591,13 @@
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" t="s">
         <v>23</v>
-      </c>
-      <c r="E52" t="s">
-        <v>24</v>
       </c>
       <c r="F52">
         <v>13228</v>
@@ -2624,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
@@ -2665,7 +2665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2673,13 +2673,13 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" t="s">
         <v>36</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>37</v>
-      </c>
-      <c r="E54" t="s">
-        <v>38</v>
       </c>
       <c r="F54">
         <v>1336540</v>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2714,13 +2714,13 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D55" t="s">
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F55">
         <v>17642866</v>
@@ -2747,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2755,13 +2755,13 @@
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
         <v>19</v>
-      </c>
-      <c r="E56" t="s">
-        <v>20</v>
       </c>
       <c r="F56">
         <v>6404186</v>
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2796,13 +2796,13 @@
         <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" t="s">
         <v>21</v>
-      </c>
-      <c r="E57" t="s">
-        <v>22</v>
       </c>
       <c r="F57">
         <v>498440</v>
@@ -2829,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2837,13 +2837,13 @@
         <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D58" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" t="s">
         <v>23</v>
-      </c>
-      <c r="E58" t="s">
-        <v>24</v>
       </c>
       <c r="F58">
         <v>79530</v>
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2878,13 +2878,13 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F59">
         <v>723404</v>
@@ -2911,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2919,13 +2919,13 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" t="s">
         <v>19</v>
-      </c>
-      <c r="E60" t="s">
-        <v>20</v>
       </c>
       <c r="F60">
         <v>402790</v>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2960,13 +2960,13 @@
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D61" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" t="s">
         <v>21</v>
-      </c>
-      <c r="E61" t="s">
-        <v>22</v>
       </c>
       <c r="F61">
         <v>2240</v>
@@ -2993,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2021</v>
       </c>
@@ -3001,13 +3001,13 @@
         <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" t="s">
         <v>23</v>
-      </c>
-      <c r="E62" t="s">
-        <v>24</v>
       </c>
       <c r="F62">
         <v>5590</v>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2021</v>
       </c>
@@ -3042,13 +3042,13 @@
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F63">
         <v>56279</v>
@@ -3075,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2021</v>
       </c>
@@ -3083,13 +3083,13 @@
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D64" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" t="s">
         <v>19</v>
-      </c>
-      <c r="E64" t="s">
-        <v>20</v>
       </c>
       <c r="F64">
         <v>7010</v>
@@ -3116,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2021</v>
       </c>
@@ -3124,13 +3124,13 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" t="s">
         <v>23</v>
-      </c>
-      <c r="E65" t="s">
-        <v>24</v>
       </c>
       <c r="F65">
         <v>7084</v>

</xml_diff>